<commit_message>
Database input data fixed
</commit_message>
<xml_diff>
--- a/CarDealersSystem/Excell Reports/Report.xlsx
+++ b/CarDealersSystem/Excell Reports/Report.xlsx
@@ -375,7 +375,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:C13"/>
   <sheetViews>
     <sheetView workbookViewId="0" rightToLeft="false">
       <selection activeCell="H11" sqref="H11"/>
@@ -450,6 +450,159 @@
         </is>
       </c>
     </row>
+    <row outlineLevel="0" r="5">
+      <c r="A5" s="0" t="inlineStr">
+        <is>
+          <t>Opel Astra</t>
+        </is>
+      </c>
+      <c r="B5" s="0" t="inlineStr">
+        <is>
+          <t>Break fluid leak</t>
+        </is>
+      </c>
+      <c r="C5" s="0" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
+      </c>
+    </row>
+    <row outlineLevel="0" r="6">
+      <c r="A6" s="0" t="inlineStr">
+        <is>
+          <t>Opel Corsa</t>
+        </is>
+      </c>
+      <c r="B6" s="0" t="inlineStr">
+        <is>
+          <t>Engine problem</t>
+        </is>
+      </c>
+      <c r="C6" s="0" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
+      </c>
+    </row>
+    <row outlineLevel="0" r="7">
+      <c r="A7" s="0" t="inlineStr">
+        <is>
+          <t>Mitsubishi Space Star</t>
+        </is>
+      </c>
+      <c r="B7" s="0" t="inlineStr">
+        <is>
+          <t>Thick-Thick Steering Wheel Sounds</t>
+        </is>
+      </c>
+      <c r="C7" s="0" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+    </row>
+    <row outlineLevel="0" r="8">
+      <c r="A8" s="0" t="inlineStr">
+        <is>
+          <t>Opel Astra</t>
+        </is>
+      </c>
+      <c r="B8" s="0" t="inlineStr">
+        <is>
+          <t>Break fluid leak</t>
+        </is>
+      </c>
+      <c r="C8" s="0" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
+      </c>
+    </row>
+    <row outlineLevel="0" r="9">
+      <c r="A9" s="0" t="inlineStr">
+        <is>
+          <t>Opel Corsa</t>
+        </is>
+      </c>
+      <c r="B9" s="0" t="inlineStr">
+        <is>
+          <t>Engine problem</t>
+        </is>
+      </c>
+      <c r="C9" s="0" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
+      </c>
+    </row>
+    <row outlineLevel="0" r="10">
+      <c r="A10" s="0" t="inlineStr">
+        <is>
+          <t>Mitsubishi Space Star</t>
+        </is>
+      </c>
+      <c r="B10" s="0" t="inlineStr">
+        <is>
+          <t>Thick-Thick Steering Wheel Sounds</t>
+        </is>
+      </c>
+      <c r="C10" s="0" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+    </row>
+    <row outlineLevel="0" r="11">
+      <c r="A11" s="0" t="inlineStr">
+        <is>
+          <t>Opel Astra</t>
+        </is>
+      </c>
+      <c r="B11" s="0" t="inlineStr">
+        <is>
+          <t>Break fluid leak</t>
+        </is>
+      </c>
+      <c r="C11" s="0" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
+      </c>
+    </row>
+    <row outlineLevel="0" r="12">
+      <c r="A12" s="0" t="inlineStr">
+        <is>
+          <t>Opel Corsa</t>
+        </is>
+      </c>
+      <c r="B12" s="0" t="inlineStr">
+        <is>
+          <t>Engine problem</t>
+        </is>
+      </c>
+      <c r="C12" s="0" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
+      </c>
+    </row>
+    <row outlineLevel="0" r="13">
+      <c r="A13" s="0" t="inlineStr">
+        <is>
+          <t>Mitsubishi Space Star</t>
+        </is>
+      </c>
+      <c r="B13" s="0" t="inlineStr">
+        <is>
+          <t>Thick-Thick Steering Wheel Sounds</t>
+        </is>
+      </c>
+      <c r="C13" s="0" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -457,7 +610,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" rightToLeft="false">
       <selection activeCell="H8" sqref="H8"/>
@@ -551,6 +704,204 @@
         </is>
       </c>
     </row>
+    <row outlineLevel="0" r="5">
+      <c r="A5" s="0" t="inlineStr">
+        <is>
+          <t>Astra</t>
+        </is>
+      </c>
+      <c r="B5" s="0" t="inlineStr">
+        <is>
+          <t>Opel</t>
+        </is>
+      </c>
+      <c r="C5" s="0" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="D5" s="0" t="inlineStr">
+        <is>
+          <t>69000</t>
+        </is>
+      </c>
+    </row>
+    <row outlineLevel="0" r="6">
+      <c r="A6" s="0" t="inlineStr">
+        <is>
+          <t>Astra</t>
+        </is>
+      </c>
+      <c r="B6" s="0" t="inlineStr">
+        <is>
+          <t>Opel</t>
+        </is>
+      </c>
+      <c r="C6" s="0" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="D6" s="0" t="inlineStr">
+        <is>
+          <t>69000</t>
+        </is>
+      </c>
+    </row>
+    <row outlineLevel="0" r="7">
+      <c r="A7" s="0" t="inlineStr">
+        <is>
+          <t>Astra</t>
+        </is>
+      </c>
+      <c r="B7" s="0" t="inlineStr">
+        <is>
+          <t>Opel</t>
+        </is>
+      </c>
+      <c r="C7" s="0" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="D7" s="0" t="inlineStr">
+        <is>
+          <t>69000</t>
+        </is>
+      </c>
+    </row>
+    <row outlineLevel="0" r="8">
+      <c r="A8" s="0" t="inlineStr">
+        <is>
+          <t>Astra</t>
+        </is>
+      </c>
+      <c r="B8" s="0" t="inlineStr">
+        <is>
+          <t>Opel</t>
+        </is>
+      </c>
+      <c r="C8" s="0" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="D8" s="0" t="inlineStr">
+        <is>
+          <t>92000</t>
+        </is>
+      </c>
+    </row>
+    <row outlineLevel="0" r="9">
+      <c r="A9" s="0" t="inlineStr">
+        <is>
+          <t>Astra</t>
+        </is>
+      </c>
+      <c r="B9" s="0" t="inlineStr">
+        <is>
+          <t>Opel</t>
+        </is>
+      </c>
+      <c r="C9" s="0" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="D9" s="0" t="inlineStr">
+        <is>
+          <t>92000</t>
+        </is>
+      </c>
+    </row>
+    <row outlineLevel="0" r="10">
+      <c r="A10" s="0" t="inlineStr">
+        <is>
+          <t>Astra</t>
+        </is>
+      </c>
+      <c r="B10" s="0" t="inlineStr">
+        <is>
+          <t>Opel</t>
+        </is>
+      </c>
+      <c r="C10" s="0" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="D10" s="0" t="inlineStr">
+        <is>
+          <t>92000</t>
+        </is>
+      </c>
+    </row>
+    <row outlineLevel="0" r="11">
+      <c r="A11" s="0" t="inlineStr">
+        <is>
+          <t>Corsa</t>
+        </is>
+      </c>
+      <c r="B11" s="0" t="inlineStr">
+        <is>
+          <t>Opel</t>
+        </is>
+      </c>
+      <c r="C11" s="0" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="D11" s="0" t="inlineStr">
+        <is>
+          <t>46000</t>
+        </is>
+      </c>
+    </row>
+    <row outlineLevel="0" r="12">
+      <c r="A12" s="0" t="inlineStr">
+        <is>
+          <t>Corsa</t>
+        </is>
+      </c>
+      <c r="B12" s="0" t="inlineStr">
+        <is>
+          <t>Opel</t>
+        </is>
+      </c>
+      <c r="C12" s="0" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="D12" s="0" t="inlineStr">
+        <is>
+          <t>46000</t>
+        </is>
+      </c>
+    </row>
+    <row outlineLevel="0" r="13">
+      <c r="A13" s="0" t="inlineStr">
+        <is>
+          <t>Corsa</t>
+        </is>
+      </c>
+      <c r="B13" s="0" t="inlineStr">
+        <is>
+          <t>Opel</t>
+        </is>
+      </c>
+      <c r="C13" s="0" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="D13" s="0" t="inlineStr">
+        <is>
+          <t>46000</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Reports data added. Excell reporter fixed
</commit_message>
<xml_diff>
--- a/CarDealersSystem/Excell Reports/Report.xlsx
+++ b/CarDealersSystem/Excell Reports/Report.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
   </bookViews>
   <sheets>
     <sheet name="Bugs" sheetId="1" r:id="rId1"/>
@@ -375,10 +375,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac">
-  <dimension ref="A1:C13"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView workbookViewId="0" rightToLeft="false">
-      <selection activeCell="H11" sqref="H11"/>
+    <sheetView tabSelected="1" workbookViewId="0" rightToLeft="false">
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -450,159 +450,6 @@
         </is>
       </c>
     </row>
-    <row outlineLevel="0" r="5">
-      <c r="A5" s="0" t="inlineStr">
-        <is>
-          <t>Opel Astra</t>
-        </is>
-      </c>
-      <c r="B5" s="0" t="inlineStr">
-        <is>
-          <t>Break fluid leak</t>
-        </is>
-      </c>
-      <c r="C5" s="0" t="inlineStr">
-        <is>
-          <t>10</t>
-        </is>
-      </c>
-    </row>
-    <row outlineLevel="0" r="6">
-      <c r="A6" s="0" t="inlineStr">
-        <is>
-          <t>Opel Corsa</t>
-        </is>
-      </c>
-      <c r="B6" s="0" t="inlineStr">
-        <is>
-          <t>Engine problem</t>
-        </is>
-      </c>
-      <c r="C6" s="0" t="inlineStr">
-        <is>
-          <t>10</t>
-        </is>
-      </c>
-    </row>
-    <row outlineLevel="0" r="7">
-      <c r="A7" s="0" t="inlineStr">
-        <is>
-          <t>Mitsubishi Space Star</t>
-        </is>
-      </c>
-      <c r="B7" s="0" t="inlineStr">
-        <is>
-          <t>Thick-Thick Steering Wheel Sounds</t>
-        </is>
-      </c>
-      <c r="C7" s="0" t="inlineStr">
-        <is>
-          <t>4</t>
-        </is>
-      </c>
-    </row>
-    <row outlineLevel="0" r="8">
-      <c r="A8" s="0" t="inlineStr">
-        <is>
-          <t>Opel Astra</t>
-        </is>
-      </c>
-      <c r="B8" s="0" t="inlineStr">
-        <is>
-          <t>Break fluid leak</t>
-        </is>
-      </c>
-      <c r="C8" s="0" t="inlineStr">
-        <is>
-          <t>10</t>
-        </is>
-      </c>
-    </row>
-    <row outlineLevel="0" r="9">
-      <c r="A9" s="0" t="inlineStr">
-        <is>
-          <t>Opel Corsa</t>
-        </is>
-      </c>
-      <c r="B9" s="0" t="inlineStr">
-        <is>
-          <t>Engine problem</t>
-        </is>
-      </c>
-      <c r="C9" s="0" t="inlineStr">
-        <is>
-          <t>10</t>
-        </is>
-      </c>
-    </row>
-    <row outlineLevel="0" r="10">
-      <c r="A10" s="0" t="inlineStr">
-        <is>
-          <t>Mitsubishi Space Star</t>
-        </is>
-      </c>
-      <c r="B10" s="0" t="inlineStr">
-        <is>
-          <t>Thick-Thick Steering Wheel Sounds</t>
-        </is>
-      </c>
-      <c r="C10" s="0" t="inlineStr">
-        <is>
-          <t>4</t>
-        </is>
-      </c>
-    </row>
-    <row outlineLevel="0" r="11">
-      <c r="A11" s="0" t="inlineStr">
-        <is>
-          <t>Opel Astra</t>
-        </is>
-      </c>
-      <c r="B11" s="0" t="inlineStr">
-        <is>
-          <t>Break fluid leak</t>
-        </is>
-      </c>
-      <c r="C11" s="0" t="inlineStr">
-        <is>
-          <t>10</t>
-        </is>
-      </c>
-    </row>
-    <row outlineLevel="0" r="12">
-      <c r="A12" s="0" t="inlineStr">
-        <is>
-          <t>Opel Corsa</t>
-        </is>
-      </c>
-      <c r="B12" s="0" t="inlineStr">
-        <is>
-          <t>Engine problem</t>
-        </is>
-      </c>
-      <c r="C12" s="0" t="inlineStr">
-        <is>
-          <t>10</t>
-        </is>
-      </c>
-    </row>
-    <row outlineLevel="0" r="13">
-      <c r="A13" s="0" t="inlineStr">
-        <is>
-          <t>Mitsubishi Space Star</t>
-        </is>
-      </c>
-      <c r="B13" s="0" t="inlineStr">
-        <is>
-          <t>Thick-Thick Steering Wheel Sounds</t>
-        </is>
-      </c>
-      <c r="C13" s="0" t="inlineStr">
-        <is>
-          <t>4</t>
-        </is>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -610,10 +457,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac">
-  <dimension ref="A1:D13"/>
+  <dimension ref="A1:D11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0" rightToLeft="false">
-      <selection activeCell="H8" sqref="H8"/>
+    <sheetView topLeftCell="A22" workbookViewId="0" rightToLeft="false">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -641,110 +488,110 @@
     <row outlineLevel="0" r="2">
       <c r="A2" s="0" t="inlineStr">
         <is>
-          <t>Astra</t>
+          <t>S7</t>
         </is>
       </c>
       <c r="B2" s="0" t="inlineStr">
         <is>
-          <t>Opel</t>
+          <t>Audi</t>
         </is>
       </c>
       <c r="C2" s="0" t="inlineStr">
         <is>
-          <t>40</t>
+          <t>7</t>
         </is>
       </c>
       <c r="D2" s="0" t="inlineStr">
         <is>
-          <t>920000</t>
+          <t>315000</t>
         </is>
       </c>
     </row>
     <row outlineLevel="0" r="3">
       <c r="A3" s="0" t="inlineStr">
         <is>
-          <t>Astra</t>
+          <t>3</t>
         </is>
       </c>
       <c r="B3" s="0" t="inlineStr">
         <is>
-          <t>Opel</t>
+          <t>Bmw</t>
         </is>
       </c>
       <c r="C3" s="0" t="inlineStr">
         <is>
-          <t>40</t>
+          <t>28</t>
         </is>
       </c>
       <c r="D3" s="0" t="inlineStr">
         <is>
-          <t>920000</t>
+          <t>896000</t>
         </is>
       </c>
     </row>
     <row outlineLevel="0" r="4">
       <c r="A4" s="0" t="inlineStr">
         <is>
-          <t>Astra</t>
+          <t>A4</t>
         </is>
       </c>
       <c r="B4" s="0" t="inlineStr">
         <is>
-          <t>Opel</t>
+          <t>Audi</t>
         </is>
       </c>
       <c r="C4" s="0" t="inlineStr">
         <is>
-          <t>40</t>
+          <t>14</t>
         </is>
       </c>
       <c r="D4" s="0" t="inlineStr">
         <is>
-          <t>920000</t>
+          <t>336000</t>
         </is>
       </c>
     </row>
     <row outlineLevel="0" r="5">
       <c r="A5" s="0" t="inlineStr">
         <is>
-          <t>Astra</t>
+          <t>Golf4</t>
         </is>
       </c>
       <c r="B5" s="0" t="inlineStr">
         <is>
-          <t>Opel</t>
+          <t>Vw</t>
         </is>
       </c>
       <c r="C5" s="0" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>35</t>
         </is>
       </c>
       <c r="D5" s="0" t="inlineStr">
         <is>
-          <t>69000</t>
+          <t>140000</t>
         </is>
       </c>
     </row>
     <row outlineLevel="0" r="6">
       <c r="A6" s="0" t="inlineStr">
         <is>
-          <t>Astra</t>
+          <t>Corolla</t>
         </is>
       </c>
       <c r="B6" s="0" t="inlineStr">
         <is>
-          <t>Opel</t>
+          <t>Toyota</t>
         </is>
       </c>
       <c r="C6" s="0" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>7</t>
         </is>
       </c>
       <c r="D6" s="0" t="inlineStr">
         <is>
-          <t>69000</t>
+          <t>56000</t>
         </is>
       </c>
     </row>
@@ -761,41 +608,41 @@
       </c>
       <c r="C7" s="0" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>14</t>
         </is>
       </c>
       <c r="D7" s="0" t="inlineStr">
         <is>
-          <t>69000</t>
+          <t>210000</t>
         </is>
       </c>
     </row>
     <row outlineLevel="0" r="8">
       <c r="A8" s="0" t="inlineStr">
         <is>
-          <t>Astra</t>
+          <t>407</t>
         </is>
       </c>
       <c r="B8" s="0" t="inlineStr">
         <is>
-          <t>Opel</t>
+          <t>Pegeout</t>
         </is>
       </c>
       <c r="C8" s="0" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>14</t>
         </is>
       </c>
       <c r="D8" s="0" t="inlineStr">
         <is>
-          <t>92000</t>
+          <t>126000</t>
         </is>
       </c>
     </row>
     <row outlineLevel="0" r="9">
       <c r="A9" s="0" t="inlineStr">
         <is>
-          <t>Astra</t>
+          <t>Corsa</t>
         </is>
       </c>
       <c r="B9" s="0" t="inlineStr">
@@ -805,100 +652,56 @@
       </c>
       <c r="C9" s="0" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>7</t>
         </is>
       </c>
       <c r="D9" s="0" t="inlineStr">
         <is>
-          <t>92000</t>
+          <t>31500</t>
         </is>
       </c>
     </row>
     <row outlineLevel="0" r="10">
       <c r="A10" s="0" t="inlineStr">
         <is>
-          <t>Astra</t>
+          <t>206</t>
         </is>
       </c>
       <c r="B10" s="0" t="inlineStr">
         <is>
-          <t>Opel</t>
+          <t>Pegeout</t>
         </is>
       </c>
       <c r="C10" s="0" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>14</t>
         </is>
       </c>
       <c r="D10" s="0" t="inlineStr">
         <is>
-          <t>92000</t>
+          <t>49000</t>
         </is>
       </c>
     </row>
     <row outlineLevel="0" r="11">
       <c r="A11" s="0" t="inlineStr">
         <is>
-          <t>Corsa</t>
+          <t>80</t>
         </is>
       </c>
       <c r="B11" s="0" t="inlineStr">
         <is>
-          <t>Opel</t>
+          <t>Audi</t>
         </is>
       </c>
       <c r="C11" s="0" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>28</t>
         </is>
       </c>
       <c r="D11" s="0" t="inlineStr">
         <is>
-          <t>46000</t>
-        </is>
-      </c>
-    </row>
-    <row outlineLevel="0" r="12">
-      <c r="A12" s="0" t="inlineStr">
-        <is>
-          <t>Corsa</t>
-        </is>
-      </c>
-      <c r="B12" s="0" t="inlineStr">
-        <is>
-          <t>Opel</t>
-        </is>
-      </c>
-      <c r="C12" s="0" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="D12" s="0" t="inlineStr">
-        <is>
-          <t>46000</t>
-        </is>
-      </c>
-    </row>
-    <row outlineLevel="0" r="13">
-      <c r="A13" s="0" t="inlineStr">
-        <is>
-          <t>Corsa</t>
-        </is>
-      </c>
-      <c r="B13" s="0" t="inlineStr">
-        <is>
-          <t>Opel</t>
-        </is>
-      </c>
-      <c r="C13" s="0" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="D13" s="0" t="inlineStr">
-        <is>
-          <t>46000</t>
+          <t>70000</t>
         </is>
       </c>
     </row>

</xml_diff>